<commit_message>
feat(cli): add merge functionality
</commit_message>
<xml_diff>
--- a/tests/cli/merge/small_no_merge.xlsx
+++ b/tests/cli/merge/small_no_merge.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alee7/ucsf/git/macpie/tests/cli/merge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4A787C-6481-A148-BC1A-D2F1D8817DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E79E1C-E3E9-A841-A91A-B803C355DBEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37060" yWindow="1060" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="small_anchor" sheetId="1" r:id="rId1"/>
-    <sheet name="instr2_all_linked" sheetId="2" r:id="rId2"/>
-    <sheet name="instr3_all_linked" sheetId="3" r:id="rId3"/>
-    <sheet name="_fields_available" sheetId="4" r:id="rId4"/>
-    <sheet name="_log_dataobjects" sheetId="5" r:id="rId5"/>
-    <sheet name="_log_operations" sheetId="6" r:id="rId6"/>
-    <sheet name="_cli_info" sheetId="7" r:id="rId7"/>
-    <sheet name="_system_info" sheetId="8" r:id="rId8"/>
+    <sheet name="_merge_info" sheetId="9" r:id="rId1"/>
+    <sheet name="small_anchor" sheetId="1" r:id="rId2"/>
+    <sheet name="instr2_all_linked" sheetId="2" r:id="rId3"/>
+    <sheet name="instr3_all_linked" sheetId="3" r:id="rId4"/>
+    <sheet name="_fields_available" sheetId="8" r:id="rId5"/>
+    <sheet name="_log_dataobjects" sheetId="4" r:id="rId6"/>
+    <sheet name="_log_operations" sheetId="5" r:id="rId7"/>
+    <sheet name="_cli_info" sheetId="6" r:id="rId8"/>
+    <sheet name="_system_info" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="236">
   <si>
     <t>PIDN</t>
   </si>
@@ -536,193 +537,205 @@
     <t>Col154</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>id_col</t>
+  </si>
+  <si>
+    <t>date_col</t>
+  </si>
+  <si>
+    <t>id2_col</t>
+  </si>
+  <si>
+    <t>filepath</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>cols</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>/Users/alee7/ucsf/git/macpie/tests/cli/link/small.xlsx</t>
+  </si>
+  <si>
+    <t>instr2_all</t>
+  </si>
+  <si>
+    <t>/Users/alee7/ucsf/git/macpie/tests/data/instr2_all.csv</t>
+  </si>
+  <si>
+    <t>instr3_all</t>
+  </si>
+  <si>
+    <t>/Users/alee7/ucsf/git/macpie/tests/data/instr3_all.csv</t>
+  </si>
+  <si>
+    <t>left_operand</t>
+  </si>
+  <si>
+    <t>right_operand</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>operation_params</t>
+  </si>
+  <si>
+    <t>operation_results_shape</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>group_by_keep_one</t>
+  </si>
+  <si>
+    <t>{'group_by_col': 'PIDN', 'date_col': 'DCDate', 'keep': 'all', 'id_col': 'InstrID', 'drop_duplicates': False}</t>
+  </si>
+  <si>
+    <t>(24, 60)</t>
+  </si>
+  <si>
+    <t>date_proximity</t>
+  </si>
+  <si>
+    <t>{'id_left_on': 'PIDN', 'id_right_on': 'PIDN', 'date_left_on': 'DCDate', 'date_right_on': 'DCDate', 'get': 'all', 'when': 'earlier_or_later', 'days': 90, 'left_link_id': 'InstrID'}</t>
+  </si>
+  <si>
+    <t>(24, 22)</t>
+  </si>
+  <si>
+    <t>(24, 164)</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>param_type</t>
+  </si>
+  <si>
+    <t>param_name</t>
+  </si>
+  <si>
+    <t>param_value</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>verbose</t>
+  </si>
+  <si>
+    <t>instrid</t>
+  </si>
+  <si>
+    <t>dcdate</t>
+  </si>
+  <si>
+    <t>pidn</t>
+  </si>
+  <si>
+    <t>primary_keep</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>secondary_get</t>
+  </si>
+  <si>
+    <t>secondary_days</t>
+  </si>
+  <si>
+    <t>secondary_when</t>
+  </si>
+  <si>
+    <t>earlier_or_later</t>
+  </si>
+  <si>
+    <t>secondary_id_col</t>
+  </si>
+  <si>
+    <t>secondary_date_col</t>
+  </si>
+  <si>
+    <t>secondary_id2_col</t>
+  </si>
+  <si>
+    <t>merge_results</t>
+  </si>
+  <si>
+    <t>keep_original</t>
+  </si>
+  <si>
+    <t>argument</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>python_version</t>
+  </si>
+  <si>
+    <t>3.8.5</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>macOS-10.15.7-x86_64-i386-64bit</t>
+  </si>
+  <si>
+    <t>computer_network_name</t>
+  </si>
+  <si>
+    <t>MAC-24HJGH5-LT</t>
+  </si>
+  <si>
+    <t>macpie_version</t>
+  </si>
+  <si>
     <t>DataObject</t>
   </si>
   <si>
     <t>Field</t>
   </si>
   <si>
-    <t>To_Merge? (enter "x")</t>
-  </si>
-  <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>instr2_all</t>
-  </si>
-  <si>
-    <t>instr3_all</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>id_col</t>
-  </si>
-  <si>
-    <t>date_col</t>
-  </si>
-  <si>
-    <t>id2_col</t>
-  </si>
-  <si>
-    <t>filepath</t>
-  </si>
-  <si>
-    <t>rows</t>
-  </si>
-  <si>
-    <t>cols</t>
-  </si>
-  <si>
-    <t>/Users/alee7/ucsf/git/macpie/tests/cli/link/small.xlsx</t>
-  </si>
-  <si>
-    <t>/Users/alee7/ucsf/git/macpie/tests/data/instr2_all.csv</t>
-  </si>
-  <si>
-    <t>/Users/alee7/ucsf/git/macpie/tests/data/instr3_all.csv</t>
-  </si>
-  <si>
-    <t>left_operand</t>
-  </si>
-  <si>
-    <t>right_operand</t>
-  </si>
-  <si>
-    <t>operation</t>
-  </si>
-  <si>
-    <t>operation_params</t>
-  </si>
-  <si>
-    <t>operation_results_shape</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>group_by_keep_one</t>
-  </si>
-  <si>
-    <t>{'group_by_col': 'PIDN', 'date_col': 'DCDate', 'keep': 'all', 'id_col': 'InstrID', 'drop_duplicates': False}</t>
-  </si>
-  <si>
-    <t>(24, 60)</t>
-  </si>
-  <si>
-    <t>date_proximity</t>
-  </si>
-  <si>
-    <t>{'id_left_on': 'PIDN', 'id_right_on': 'PIDN', 'date_left_on': 'DCDate', 'date_right_on': 'DCDate', 'get': 'all', 'when': 'earlier_or_later', 'days': 90, 'left_link_id': 'InstrID'}</t>
-  </si>
-  <si>
-    <t>(24, 22)</t>
-  </si>
-  <si>
-    <t>(24, 164)</t>
-  </si>
-  <si>
-    <t>command</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>param_type</t>
-  </si>
-  <si>
-    <t>param_name</t>
-  </si>
-  <si>
-    <t>param_value</t>
-  </si>
-  <si>
-    <t>link</t>
-  </si>
-  <si>
-    <t>0.1.0</t>
-  </si>
-  <si>
-    <t>option</t>
-  </si>
-  <si>
-    <t>verbose</t>
-  </si>
-  <si>
-    <t>instrid</t>
-  </si>
-  <si>
-    <t>dcdate</t>
-  </si>
-  <si>
-    <t>pidn</t>
-  </si>
-  <si>
-    <t>primary_keep</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>secondary_get</t>
-  </si>
-  <si>
-    <t>secondary_days</t>
-  </si>
-  <si>
-    <t>secondary_when</t>
-  </si>
-  <si>
-    <t>earlier_or_later</t>
-  </si>
-  <si>
-    <t>secondary_id_col</t>
-  </si>
-  <si>
-    <t>secondary_date_col</t>
-  </si>
-  <si>
-    <t>secondary_id2_col</t>
-  </si>
-  <si>
-    <t>merge_results</t>
-  </si>
-  <si>
-    <t>keep_original</t>
-  </si>
-  <si>
-    <t>argument</t>
-  </si>
-  <si>
-    <t>primary</t>
-  </si>
-  <si>
-    <t>secondary</t>
-  </si>
-  <si>
-    <t>python_version</t>
-  </si>
-  <si>
-    <t>3.8.5</t>
-  </si>
-  <si>
-    <t>platform</t>
-  </si>
-  <si>
-    <t>macOS-10.15.7-x86_64-i386-64bit</t>
-  </si>
-  <si>
-    <t>computer_network_name</t>
-  </si>
-  <si>
-    <t>MAC-24HJGH5-LT</t>
-  </si>
-  <si>
-    <t>macpie_version</t>
-  </si>
-  <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>merged</t>
+  </si>
+  <si>
+    <t>Merge?</t>
+  </si>
+  <si>
+    <t>{"name": "small", "id_col": "InstrID", "date_col": "DCDate", "id2_col": "PIDN", "filepath": "/Users/alee7/ucsf/git/macpie/tests/cli/link/small.xlsx", "rows": 24, "cols": 60}</t>
+  </si>
+  <si>
+    <t>["instr2_all", "instr3_all"]</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -781,12 +794,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,6 +1102,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353D019A-8068-1644-A9B9-B6B9A841EE9F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="120.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH25"/>
   <sheetViews>
@@ -5512,7 +5577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V25"/>
   <sheetViews>
@@ -6277,7 +6342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:FH25"/>
   <sheetViews>
@@ -10063,94 +10128,96 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA6E69A-E84B-A140-B1BF-098424845A44}">
   <dimension ref="A1:C238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>228</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -10158,7 +10225,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -10166,7 +10233,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -10174,7 +10241,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -10182,7 +10249,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -10190,7 +10257,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -10198,7 +10265,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -10206,7 +10273,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -10214,7 +10281,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -10222,7 +10289,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -10230,7 +10297,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -10238,7 +10305,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -10246,7 +10313,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -10254,7 +10321,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -10262,7 +10329,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -10270,7 +10337,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -10278,7 +10345,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -10286,7 +10353,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -10294,7 +10361,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -10302,7 +10369,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -10310,7 +10377,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -10318,7 +10385,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -10326,7 +10393,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -10334,7 +10401,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -10342,7 +10409,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -10350,7 +10417,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -10358,7 +10425,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -10366,7 +10433,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -10374,7 +10441,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -10382,7 +10449,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -10390,7 +10457,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -10398,7 +10465,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -10406,7 +10473,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -10414,7 +10481,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -10422,7 +10489,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -10430,7 +10497,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -10438,7 +10505,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -10446,7 +10513,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -10454,7 +10521,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -10462,7 +10529,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
@@ -10470,7 +10537,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -10478,7 +10545,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
@@ -10486,7 +10553,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
@@ -10494,7 +10561,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
@@ -10502,7 +10569,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B52" t="s">
         <v>53</v>
@@ -10510,7 +10577,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
@@ -10518,7 +10585,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B54" t="s">
         <v>55</v>
@@ -10526,7 +10593,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
@@ -10534,7 +10601,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
         <v>57</v>
@@ -10542,7 +10609,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B57" t="s">
         <v>58</v>
@@ -10550,7 +10617,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B58" t="s">
         <v>59</v>
@@ -10558,86 +10625,95 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B59" t="s">
         <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
       </c>
+      <c r="C60" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B61" t="s">
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
       </c>
+      <c r="C66" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -10645,7 +10721,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B68" t="s">
         <v>11</v>
@@ -10653,7 +10729,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
@@ -10661,7 +10737,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B70" t="s">
         <v>13</v>
@@ -10669,7 +10745,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B71" t="s">
         <v>14</v>
@@ -10677,7 +10753,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s">
         <v>15</v>
@@ -10685,7 +10761,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B73" t="s">
         <v>16</v>
@@ -10693,7 +10769,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B74" t="s">
         <v>17</v>
@@ -10701,7 +10777,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B75" t="s">
         <v>65</v>
@@ -10709,7 +10785,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B76" t="s">
         <v>66</v>
@@ -10717,7 +10793,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B77" t="s">
         <v>67</v>
@@ -10725,78 +10801,84 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B78" t="s">
         <v>0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B79" t="s">
         <v>3</v>
       </c>
+      <c r="C79" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B80" t="s">
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B84" t="s">
         <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -10804,7 +10886,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B86" t="s">
         <v>10</v>
@@ -10812,7 +10894,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B87" t="s">
         <v>11</v>
@@ -10820,7 +10902,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B88" t="s">
         <v>12</v>
@@ -10828,7 +10910,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B89" t="s">
         <v>13</v>
@@ -10836,7 +10918,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B90" t="s">
         <v>14</v>
@@ -10844,7 +10926,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B91" t="s">
         <v>15</v>
@@ -10852,7 +10934,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B92" t="s">
         <v>16</v>
@@ -10860,7 +10942,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B93" t="s">
         <v>17</v>
@@ -10868,7 +10950,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B94" t="s">
         <v>18</v>
@@ -10876,7 +10958,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s">
         <v>19</v>
@@ -10884,7 +10966,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B96" t="s">
         <v>20</v>
@@ -10892,7 +10974,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B97" t="s">
         <v>21</v>
@@ -10900,7 +10982,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B98" t="s">
         <v>22</v>
@@ -10908,7 +10990,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B99" t="s">
         <v>23</v>
@@ -10916,7 +10998,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B100" t="s">
         <v>24</v>
@@ -10924,7 +11006,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B101" t="s">
         <v>25</v>
@@ -10932,7 +11014,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B102" t="s">
         <v>26</v>
@@ -10940,7 +11022,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B103" t="s">
         <v>27</v>
@@ -10948,7 +11030,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B104" t="s">
         <v>28</v>
@@ -10956,7 +11038,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B105" t="s">
         <v>29</v>
@@ -10964,7 +11046,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B106" t="s">
         <v>30</v>
@@ -10972,7 +11054,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B107" t="s">
         <v>31</v>
@@ -10980,7 +11062,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B108" t="s">
         <v>32</v>
@@ -10988,7 +11070,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B109" t="s">
         <v>33</v>
@@ -10996,7 +11078,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B110" t="s">
         <v>34</v>
@@ -11004,7 +11086,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B111" t="s">
         <v>35</v>
@@ -11012,7 +11094,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B112" t="s">
         <v>36</v>
@@ -11020,7 +11102,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B113" t="s">
         <v>37</v>
@@ -11028,7 +11110,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B114" t="s">
         <v>38</v>
@@ -11036,7 +11118,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B115" t="s">
         <v>39</v>
@@ -11044,7 +11126,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B116" t="s">
         <v>40</v>
@@ -11052,7 +11134,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B117" t="s">
         <v>41</v>
@@ -11060,7 +11142,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B118" t="s">
         <v>42</v>
@@ -11068,7 +11150,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B119" t="s">
         <v>43</v>
@@ -11076,7 +11158,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B120" t="s">
         <v>44</v>
@@ -11084,7 +11166,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B121" t="s">
         <v>45</v>
@@ -11092,7 +11174,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B122" t="s">
         <v>46</v>
@@ -11100,7 +11182,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B123" t="s">
         <v>47</v>
@@ -11108,7 +11190,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B124" t="s">
         <v>48</v>
@@ -11116,7 +11198,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B125" t="s">
         <v>49</v>
@@ -11124,7 +11206,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B126" t="s">
         <v>50</v>
@@ -11132,7 +11214,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B127" t="s">
         <v>51</v>
@@ -11140,7 +11222,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B128" t="s">
         <v>52</v>
@@ -11148,7 +11230,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B129" t="s">
         <v>53</v>
@@ -11156,7 +11238,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B130" t="s">
         <v>54</v>
@@ -11164,7 +11246,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B131" t="s">
         <v>55</v>
@@ -11172,7 +11254,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B132" t="s">
         <v>56</v>
@@ -11180,7 +11262,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B133" t="s">
         <v>57</v>
@@ -11188,7 +11270,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B134" t="s">
         <v>58</v>
@@ -11196,7 +11278,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B135" t="s">
         <v>59</v>
@@ -11204,7 +11286,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B136" t="s">
         <v>69</v>
@@ -11212,7 +11294,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B137" t="s">
         <v>70</v>
@@ -11220,7 +11302,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B138" t="s">
         <v>71</v>
@@ -11228,7 +11310,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B139" t="s">
         <v>72</v>
@@ -11236,7 +11318,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B140" t="s">
         <v>73</v>
@@ -11244,7 +11326,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B141" t="s">
         <v>74</v>
@@ -11252,7 +11334,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B142" t="s">
         <v>75</v>
@@ -11260,7 +11342,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B143" t="s">
         <v>76</v>
@@ -11268,7 +11350,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B144" t="s">
         <v>77</v>
@@ -11276,7 +11358,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B145" t="s">
         <v>78</v>
@@ -11284,7 +11366,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B146" t="s">
         <v>79</v>
@@ -11292,7 +11374,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B147" t="s">
         <v>80</v>
@@ -11300,7 +11382,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B148" t="s">
         <v>81</v>
@@ -11308,7 +11390,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B149" t="s">
         <v>82</v>
@@ -11316,7 +11398,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B150" t="s">
         <v>83</v>
@@ -11324,7 +11406,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B151" t="s">
         <v>84</v>
@@ -11332,7 +11414,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B152" t="s">
         <v>85</v>
@@ -11340,7 +11422,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B153" t="s">
         <v>86</v>
@@ -11348,7 +11430,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B154" t="s">
         <v>87</v>
@@ -11356,7 +11438,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B155" t="s">
         <v>88</v>
@@ -11364,7 +11446,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B156" t="s">
         <v>89</v>
@@ -11372,7 +11454,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B157" t="s">
         <v>90</v>
@@ -11380,7 +11462,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B158" t="s">
         <v>91</v>
@@ -11388,7 +11470,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B159" t="s">
         <v>92</v>
@@ -11396,7 +11478,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B160" t="s">
         <v>93</v>
@@ -11404,7 +11486,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B161" t="s">
         <v>94</v>
@@ -11412,7 +11494,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B162" t="s">
         <v>95</v>
@@ -11420,7 +11502,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B163" t="s">
         <v>96</v>
@@ -11428,7 +11510,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B164" t="s">
         <v>97</v>
@@ -11436,7 +11518,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B165" t="s">
         <v>98</v>
@@ -11444,7 +11526,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B166" t="s">
         <v>99</v>
@@ -11452,7 +11534,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B167" t="s">
         <v>100</v>
@@ -11460,7 +11542,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B168" t="s">
         <v>101</v>
@@ -11468,7 +11550,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B169" t="s">
         <v>102</v>
@@ -11476,7 +11558,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B170" t="s">
         <v>103</v>
@@ -11484,7 +11566,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B171" t="s">
         <v>104</v>
@@ -11492,7 +11574,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B172" t="s">
         <v>105</v>
@@ -11500,7 +11582,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B173" t="s">
         <v>106</v>
@@ -11508,7 +11590,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B174" t="s">
         <v>107</v>
@@ -11516,7 +11598,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B175" t="s">
         <v>108</v>
@@ -11524,7 +11606,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B176" t="s">
         <v>109</v>
@@ -11532,7 +11614,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B177" t="s">
         <v>110</v>
@@ -11540,7 +11622,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B178" t="s">
         <v>111</v>
@@ -11548,7 +11630,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B179" t="s">
         <v>112</v>
@@ -11556,7 +11638,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B180" t="s">
         <v>113</v>
@@ -11564,7 +11646,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B181" t="s">
         <v>114</v>
@@ -11572,7 +11654,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B182" t="s">
         <v>115</v>
@@ -11580,7 +11662,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B183" t="s">
         <v>116</v>
@@ -11588,7 +11670,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B184" t="s">
         <v>117</v>
@@ -11596,7 +11678,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B185" t="s">
         <v>118</v>
@@ -11604,7 +11686,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B186" t="s">
         <v>119</v>
@@ -11612,7 +11694,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B187" t="s">
         <v>120</v>
@@ -11620,7 +11702,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B188" t="s">
         <v>121</v>
@@ -11628,7 +11710,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B189" t="s">
         <v>122</v>
@@ -11636,7 +11718,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B190" t="s">
         <v>123</v>
@@ -11644,7 +11726,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B191" t="s">
         <v>124</v>
@@ -11652,7 +11734,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B192" t="s">
         <v>125</v>
@@ -11660,7 +11742,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B193" t="s">
         <v>126</v>
@@ -11668,7 +11750,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B194" t="s">
         <v>127</v>
@@ -11676,7 +11758,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B195" t="s">
         <v>128</v>
@@ -11684,7 +11766,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B196" t="s">
         <v>129</v>
@@ -11692,7 +11774,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B197" t="s">
         <v>130</v>
@@ -11700,7 +11782,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B198" t="s">
         <v>131</v>
@@ -11708,7 +11790,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B199" t="s">
         <v>132</v>
@@ -11716,7 +11798,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B200" t="s">
         <v>133</v>
@@ -11724,7 +11806,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B201" t="s">
         <v>134</v>
@@ -11732,7 +11814,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B202" t="s">
         <v>135</v>
@@ -11740,7 +11822,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B203" t="s">
         <v>136</v>
@@ -11748,7 +11830,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B204" t="s">
         <v>137</v>
@@ -11756,7 +11838,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B205" t="s">
         <v>138</v>
@@ -11764,7 +11846,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B206" t="s">
         <v>139</v>
@@ -11772,7 +11854,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B207" t="s">
         <v>140</v>
@@ -11780,7 +11862,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B208" t="s">
         <v>141</v>
@@ -11788,7 +11870,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B209" t="s">
         <v>142</v>
@@ -11796,7 +11878,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B210" t="s">
         <v>143</v>
@@ -11804,7 +11886,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B211" t="s">
         <v>144</v>
@@ -11812,7 +11894,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B212" t="s">
         <v>145</v>
@@ -11820,7 +11902,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B213" t="s">
         <v>146</v>
@@ -11828,7 +11910,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B214" t="s">
         <v>147</v>
@@ -11836,7 +11918,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B215" t="s">
         <v>148</v>
@@ -11844,7 +11926,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B216" t="s">
         <v>149</v>
@@ -11852,7 +11934,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B217" t="s">
         <v>150</v>
@@ -11860,7 +11942,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B218" t="s">
         <v>151</v>
@@ -11868,7 +11950,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B219" t="s">
         <v>152</v>
@@ -11876,7 +11958,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B220" t="s">
         <v>153</v>
@@ -11884,7 +11966,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B221" t="s">
         <v>154</v>
@@ -11892,7 +11974,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B222" t="s">
         <v>155</v>
@@ -11900,7 +11982,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B223" t="s">
         <v>156</v>
@@ -11908,7 +11990,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B224" t="s">
         <v>157</v>
@@ -11916,7 +11998,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B225" t="s">
         <v>158</v>
@@ -11924,7 +12006,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B226" t="s">
         <v>159</v>
@@ -11932,7 +12014,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B227" t="s">
         <v>160</v>
@@ -11940,7 +12022,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B228" t="s">
         <v>161</v>
@@ -11948,7 +12030,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B229" t="s">
         <v>162</v>
@@ -11956,7 +12038,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B230" t="s">
         <v>163</v>
@@ -11964,7 +12046,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B231" t="s">
         <v>164</v>
@@ -11972,7 +12054,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B232" t="s">
         <v>165</v>
@@ -11980,7 +12062,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B233" t="s">
         <v>166</v>
@@ -11988,7 +12070,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B234" t="s">
         <v>167</v>
@@ -11996,7 +12078,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B235" t="s">
         <v>168</v>
@@ -12004,7 +12086,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B236" t="s">
         <v>65</v>
@@ -12012,7 +12094,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B237" t="s">
         <v>66</v>
@@ -12020,7 +12102,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B238" t="s">
         <v>67</v>
@@ -12031,11 +12113,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12049,30 +12133,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -12084,7 +12168,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -12095,7 +12179,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -12107,7 +12191,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F3">
         <v>8955</v>
@@ -12118,7 +12202,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -12130,7 +12214,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F4">
         <v>9377</v>
@@ -12144,8 +12228,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12161,70 +12245,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
         <v>190</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" t="s">
         <v>194</v>
-      </c>
-      <c r="D4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E4" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -12232,8 +12316,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12242,33 +12326,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" t="s">
         <v>203</v>
-      </c>
-      <c r="B2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" t="s">
-        <v>206</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -12276,101 +12360,101 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" t="s">
         <v>204</v>
-      </c>
-      <c r="C3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" t="s">
         <v>205</v>
-      </c>
-      <c r="D4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E4" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E8">
         <v>90</v>
@@ -12378,84 +12462,84 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10" t="s">
         <v>204</v>
-      </c>
-      <c r="C10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E10" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E11" t="s">
         <v>205</v>
-      </c>
-      <c r="D11" t="s">
-        <v>217</v>
-      </c>
-      <c r="E11" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -12463,16 +12547,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D14" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -12480,53 +12564,53 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E15" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D16" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C17" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E17" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -12534,8 +12618,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12544,42 +12628,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>